<commit_message>
Summarized more articles, added references
</commit_message>
<xml_diff>
--- a/Organized/References.xlsx
+++ b/Organized/References.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeta\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Desktop\Software Research\Software-Research-Project\Organized\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -74,6 +74,25 @@
     <t>*discovery (page views, unique users, popular content)
 *usage (ratio: usage to discovery rate)
 *retention (commits per user)</t>
+  </si>
+  <si>
+    <t>Zephyr</t>
+  </si>
+  <si>
+    <t>QA Metrics The Value of Testing Metrics Within Software Development</t>
+  </si>
+  <si>
+    <t>https://www.getzephyr.com/sites/default/files/content/resources/QA%20Metrics%20The%20Value%20of%20Testing%20Metrics%20Within%20Software%20Development%20DNLD.pdf</t>
+  </si>
+  <si>
+    <t>*requirements and requirement coverage
+*defect distribution
+*defect open and close rate
+*execution trend
+*MTTD
+*MTTR
+*Defect Removal Efficiency
+*Customer Reported Issue Percentage</t>
   </si>
 </sst>
 </file>
@@ -149,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -164,6 +183,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -446,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,6 +549,23 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3">
+        <v>42278</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated references and summarized article
</commit_message>
<xml_diff>
--- a/Organized/References.xlsx
+++ b/Organized/References.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Desktop\Software Research\Software-Research-Project\Organized\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeta\Desktop\Research\Software-Research-Project\Organized\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -93,6 +93,27 @@
 *MTTR
 *Defect Removal Efficiency
 *Customer Reported Issue Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metrics for Measuring the Quality of Object-Oriented Software
+</t>
+  </si>
+  <si>
+    <t>Gagandeep Singh</t>
+  </si>
+  <si>
+    <t>http://delivery.acm.org.libproxy.auc.ca/10.1145/2510000/2507311/p66b-singh.pdf?ip=199.212.55.169&amp;id=2507311&amp;acc=ACTIVE%20SERVICE&amp;key=FD0067F557510FFB%2E2E114FAB5F912086%2E4D4702B0C3E38B35%2E4D4702B0C3E38B35&amp;CFID=939957675&amp;CFTOKEN=22411919&amp;__acm__=1495551123_66186ebadebfcf7a06c0c6f881edc6c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*LOC (lines of code) - understandability 
+*CC (cyclomatic complexity) - complexity
+*CBO (coupling between objects) - efficiency, reuse, complexity
+*LCOM (lack of cohesion) - reuse, complexity
+*WMC (weighted methods per class) - maintainability, reuse
+*RFC (response for a class) - understandability, complexity
+*MI (maintainabiliyt index) - maintainability
+*NOC (number of children) - reuse, efficiency
+*DIT (depth of inheritance tree) - reuse, complexity </t>
   </si>
 </sst>
 </file>
@@ -468,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +501,7 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="53" customWidth="1"/>
+    <col min="5" max="5" width="59.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,6 +585,23 @@
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>41518</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved the summary of articles already complted
</commit_message>
<xml_diff>
--- a/Organized/References.xlsx
+++ b/Organized/References.xlsx
@@ -50,9 +50,6 @@
     <t>Metrics</t>
   </si>
   <si>
-    <t>*pirate metrics (community involvement)</t>
-  </si>
-  <si>
     <t>http://redmonk.com/dberkholz/2013/04/22/the-size-of-open-source-communities-and-its-impact-upon-activity-licensing-and-hosting/</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
 *Lines of Code Per Function
 *Comment Density
 *Maximum Nesting</t>
+  </si>
+  <si>
+    <t>*pirate metrics (community involvement and retention)</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,107 +570,107 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>41365</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="3">
         <v>42767</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <v>42278</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="3">
         <v>41518</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <v>39630</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3">
         <v>40422</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed old documentation, and added to summaries
</commit_message>
<xml_diff>
--- a/Organized/References.xlsx
+++ b/Organized/References.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeta\Desktop\Research\Software-Research-Project\Organized\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Title</t>
   </si>
@@ -232,6 +227,34 @@
 • OpenSource Maturity Model
 • QualOSS
 </t>
+  </si>
+  <si>
+    <t>https://www.dmst.aueb.gr/dds/pubs/conf/2008-OSS-qmodel/html/SGSS08.htm</t>
+  </si>
+  <si>
+    <t>The SQO-OSS quality model: measurement based open source software evaluation</t>
+  </si>
+  <si>
+    <t>Ioannis Samoladas, Georgios Gousios, Diomidis Spinellis and Ioannis Stamelos</t>
+  </si>
+  <si>
+    <t>The QualOSS Open Source Assessment Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martín Soto and Marcus Ciolkowski
+</t>
+  </si>
+  <si>
+    <t>https://www.rose-hulman.edu/class/csse/OldFiles/csse575/Resources/MeasOpenSource-05314237.pdf</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org.libproxy.auc.ca/citation.cfm?id=1572200&amp;CFID=951820277&amp;CFTOKEN=35034244</t>
+  </si>
+  <si>
+    <t>Introducing the OpenSource Maturity Model</t>
+  </si>
+  <si>
+    <t>Etiel Petrinja, Ranga Nambakam, Alberto Sillitti</t>
   </si>
 </sst>
 </file>
@@ -307,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -329,6 +352,15 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,7 +422,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,7 +457,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,7 +634,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -610,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,6 +825,51 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="7">
+        <v>39692</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="7">
+        <v>40087</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="7">
+        <v>39934</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated article summary and references, deleted quick notes
</commit_message>
<xml_diff>
--- a/Organized/References.xlsx
+++ b/Organized/References.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Title</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>Etiel Petrinja, Ranga Nambakam, Alberto Sillitti</t>
+  </si>
+  <si>
+    <t>• Utlizes metrics found and based on the ISO9126 guidelines (similar in respect to other models, but different in implementation)</t>
+  </si>
+  <si>
+    <t>Note: comprensive metrics for the ISO9126 can be found at http://www.arisa.se/compendium/node6.html</t>
   </si>
 </sst>
 </file>
@@ -330,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -353,14 +359,11 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,7 +637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,19 +829,21 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="7">
         <v>39692</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -853,7 +858,9 @@
       <c r="D12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -868,7 +875,14 @@
       <c r="D13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>